<commit_message>
Student Role Accepting Script completed
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Corporate Role Creation.xlsx
+++ b/Excel/PluginLive Automation Corporate Role Creation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CorporateLogin" sheetId="1" state="visible" r:id="rId3"/>
@@ -14,7 +14,6 @@
     <sheet name="Questionnaire" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="InterviewWorkflow" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="EligibilityCriteria" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="ApplyRole" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">userName</t>
   </si>
@@ -209,9 +208,6 @@
   </si>
   <si>
     <t xml:space="preserve">Javascript Frameworks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search</t>
   </si>
 </sst>
 </file>
@@ -320,7 +316,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -351,10 +347,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -888,7 +880,7 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -985,38 +977,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed the Degree and department
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation Corporate Role Creation.xlsx
+++ b/Excel/PluginLive Automation Corporate Role Creation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CorporateLogin" sheetId="1" state="visible" r:id="rId3"/>
@@ -33,10 +33,10 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">priya.t+1@icanio.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priya@2606</t>
+    <t xml:space="preserve">priya.t+corporate3@icanio.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@wH5yrm3</t>
   </si>
   <si>
     <t xml:space="preserve">function</t>
@@ -57,10 +57,10 @@
     <t xml:space="preserve">enddate</t>
   </si>
   <si>
-    <t xml:space="preserve">Quality Functions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quality Roles</t>
+    <t xml:space="preserve">Engineering &amp; Architecture </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Designer </t>
   </si>
   <si>
     <t xml:space="preserve">Please check the eligibility criteria before Applying the role</t>
@@ -186,7 +186,7 @@
     <t xml:space="preserve">year5</t>
   </si>
   <si>
-    <t xml:space="preserve">BACHELOR OF ENGINEERING </t>
+    <t xml:space="preserve">BACHELOR OF COMPUTER APPLICATIONS </t>
   </si>
   <si>
     <t xml:space="preserve">B.E - Computer Science Engineering</t>
@@ -207,7 +207,7 @@
     <t xml:space="preserve">Communication</t>
   </si>
   <si>
-    <t xml:space="preserve">Javascript Frameworks</t>
+    <t xml:space="preserve">Javascript</t>
   </si>
 </sst>
 </file>
@@ -218,7 +218,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,11 +242,24 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9.8"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
@@ -258,16 +271,15 @@
     </font>
     <font>
       <sz val="9.8"/>
-      <color rgb="FF6AAB73"/>
+      <color rgb="FFBCBEC4"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9.8"/>
-      <color rgb="FFBCBEC4"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -312,11 +324,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,8 +341,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -338,6 +350,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -345,7 +361,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -602,7 +618,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,19 +631,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="priya.t+1@icanio.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="Priya@2606"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -645,7 +657,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -674,7 +686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -684,7 +696,7 @@
       <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -725,21 +737,21 @@
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="7" t="n">
         <v>200000</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="7" t="n">
         <v>400000</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -811,7 +823,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -839,7 +851,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -880,11 +892,14 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -927,29 +942,29 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+    <row r="2" customFormat="false" ht="62" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>60</v>
       </c>
       <c r="I2" s="1" t="n">

</xml_diff>